<commit_message>
"Add API Key updater"
</commit_message>
<xml_diff>
--- a/output/1- Sample Inv.xlsx
+++ b/output/1- Sample Inv.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samuel Ehrlich\Desktop\My Drive\UI Path Toolkit\Presales Presentations\Demo Kit\InvoiceProcessingMain\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{447FFFC9-643B-417B-851F-86C445578149}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5F724E9-86F8-42CD-A8D1-674B88848976}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6000" yWindow="1380" windowWidth="11580" windowHeight="7620" xr2:uid="{C47D72FF-F093-4427-B53B-E1BE832892F7}"/>
+    <workbookView xWindow="735" yWindow="735" windowWidth="14400" windowHeight="7373" xr2:uid="{C47D72FF-F093-4427-B53B-E1BE832892F7}"/>
   </bookViews>
   <sheets>
     <sheet name="TableofData - Formatted" sheetId="5" r:id="rId1"/>

</xml_diff>